<commit_message>
edited lectures and scripts + removed data processing from the report
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -379,7 +379,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -407,36 +407,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -772,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DD11F9-8F48-D849-960C-B711504FDE7B}">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
prepping data for pca
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au763634_uni_au_dk/Documents/MappingPlants/admin/courses/2025 01 Applied statistics and R/dtu_applied_stat_R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="8_{6C75A161-9A34-8241-9516-4734A37920F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF977F66-4221-1745-894E-C883FBC1F5D0}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="8_{6C75A161-9A34-8241-9516-4734A37920F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9390C288-B0EC-5F44-9E4B-AD215C072A28}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="20500" xr2:uid="{6FC8138E-6706-3545-A1DF-0C2F42AB7A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="117">
   <si>
     <t>slides</t>
   </si>
@@ -339,6 +339,54 @@
   </si>
   <si>
     <t>predictor_type</t>
+  </si>
+  <si>
+    <t>Binary data</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Dead/Alive</t>
+  </si>
+  <si>
+    <t>Nominal (”label”, several groups)</t>
+  </si>
+  <si>
+    <t>Eye colour: Blue/ Brown / Grey / Green</t>
+  </si>
+  <si>
+    <t>Where do you live: Denmark, Germany, Sweden.</t>
+  </si>
+  <si>
+    <t>Ordinal</t>
+  </si>
+  <si>
+    <t>How do you feel today?: Very unhappy, unhappy, OK, happy, very</t>
+  </si>
+  <si>
+    <t>happy.</t>
+  </si>
+  <si>
+    <t>Do you try to eat healthily?: Never, Sometimes, Always</t>
+  </si>
+  <si>
+    <t>Interval (does have a numerical distance between values)</t>
+  </si>
+  <si>
+    <t>BMI categories (&lt;25, 25-</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>all 3 numeric</t>
+  </si>
+  <si>
+    <t>other notes</t>
+  </si>
+  <si>
+    <t>linear regrssion to simple</t>
   </si>
 </sst>
 </file>
@@ -740,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DD11F9-8F48-D849-960C-B711504FDE7B}">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J89" sqref="J89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -755,7 +803,7 @@
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="E1" t="s">
         <v>97</v>
       </c>
@@ -768,8 +816,11 @@
       <c r="H1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>0</v>
       </c>
@@ -783,7 +834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>0</v>
       </c>
@@ -797,7 +848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>0</v>
       </c>
@@ -811,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>0</v>
       </c>
@@ -822,7 +873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>0</v>
       </c>
@@ -833,7 +884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>0</v>
       </c>
@@ -844,7 +895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>0</v>
       </c>
@@ -855,7 +906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>0</v>
       </c>
@@ -866,7 +917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>0</v>
       </c>
@@ -877,7 +928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>0</v>
       </c>
@@ -887,8 +938,11 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="K11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>0</v>
       </c>
@@ -898,8 +952,11 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="K12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>0</v>
       </c>
@@ -909,8 +966,11 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="L13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>1</v>
       </c>
@@ -920,8 +980,11 @@
       <c r="C14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="L14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>1</v>
       </c>
@@ -931,8 +994,11 @@
       <c r="C15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="K15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>1</v>
       </c>
@@ -942,8 +1008,11 @@
       <c r="C16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="L16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>1</v>
       </c>
@@ -953,8 +1022,11 @@
       <c r="C17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="L17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>1</v>
       </c>
@@ -964,8 +1036,11 @@
       <c r="C18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="K18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>1</v>
       </c>
@@ -975,8 +1050,11 @@
       <c r="C19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="L19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>1</v>
       </c>
@@ -986,8 +1064,11 @@
       <c r="C20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="L20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>2</v>
       </c>
@@ -997,8 +1078,11 @@
       <c r="C21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="L21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1008,8 +1092,11 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="K22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1019,8 +1106,11 @@
       <c r="C23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="L23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1031,7 +1121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1042,7 +1132,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1053,7 +1143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1064,7 +1154,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1075,7 +1165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1086,7 +1176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1097,7 +1187,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1108,7 +1198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1119,7 +1209,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1130,7 +1220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1141,7 +1231,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1152,7 +1242,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1163,7 +1253,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1174,7 +1264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1185,7 +1275,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1196,7 +1286,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1207,7 +1297,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1218,7 +1308,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1229,7 +1319,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>4</v>
       </c>
@@ -1240,7 +1330,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>4</v>
       </c>
@@ -1251,7 +1341,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>4</v>
       </c>
@@ -1262,7 +1352,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>4</v>
       </c>
@@ -1272,8 +1362,23 @@
       <c r="C46" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46" t="s">
+        <v>114</v>
+      </c>
+      <c r="I46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>4</v>
       </c>
@@ -1284,7 +1389,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
added a skree plot for the PCA analysis
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au763634_uni_au_dk/Documents/MappingPlants/admin/courses/2025 01 Applied statistics and R/dtu_applied_stat_R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="8_{6C75A161-9A34-8241-9516-4734A37920F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9390C288-B0EC-5F44-9E4B-AD215C072A28}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="8_{6C75A161-9A34-8241-9516-4734A37920F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0544CC0A-2237-714D-8B4C-9310E59E7D6E}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="20500" xr2:uid="{6FC8138E-6706-3545-A1DF-0C2F42AB7A96}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{6FC8138E-6706-3545-A1DF-0C2F42AB7A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="119">
   <si>
     <t>slides</t>
   </si>
@@ -387,16 +387,28 @@
   </si>
   <si>
     <t>linear regrssion to simple</t>
+  </si>
+  <si>
+    <t>groupings</t>
+  </si>
+  <si>
+    <t>comparing the variance within group with the variance between the groups</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Aptos-Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Aptos-Light"/>
       <family val="2"/>
     </font>
@@ -421,8 +433,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,1214 +802,1533 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DD11F9-8F48-D849-960C-B711504FDE7B}">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:L23"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="E1" t="s">
+    <row r="1" spans="1:13">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:13">
+      <c r="A3" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
       <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
       </c>
       <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
       </c>
       <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
       </c>
       <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
       </c>
       <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:13">
+      <c r="A16" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
       </c>
       <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
       </c>
       <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
         <v>22</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
       </c>
       <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
         <v>24</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:13">
+      <c r="A24" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:13">
+      <c r="A26" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="27" spans="1:13">
+      <c r="A27" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="28" spans="1:13">
+      <c r="A28" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" spans="1:13">
+      <c r="A29" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30">
+    <row r="30" spans="1:13">
+      <c r="A30" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B30">
         <v>3</v>
       </c>
-      <c r="B30" t="s">
-        <v>0</v>
-      </c>
       <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31">
+    <row r="31" spans="1:13">
+      <c r="A31" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B31">
         <v>3</v>
       </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
       <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
-      <c r="A32">
+    <row r="32" spans="1:13">
+      <c r="A32" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B32">
         <v>3</v>
       </c>
-      <c r="B32" t="s">
-        <v>1</v>
-      </c>
       <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33">
+    <row r="33" spans="1:10">
+      <c r="A33" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B33">
         <v>3</v>
       </c>
-      <c r="B33" t="s">
-        <v>1</v>
-      </c>
       <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34">
+    <row r="34" spans="1:10">
+      <c r="A34" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B34">
         <v>3</v>
       </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
       <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35">
+    <row r="35" spans="1:10">
+      <c r="A35" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B35">
         <v>3</v>
       </c>
-      <c r="B35" t="s">
-        <v>1</v>
-      </c>
       <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36">
+    <row r="36" spans="1:10">
+      <c r="A36" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B36">
         <v>3</v>
       </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
       <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="A37">
+    <row r="37" spans="1:10">
+      <c r="A37" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B37">
         <v>3</v>
       </c>
-      <c r="B37" t="s">
-        <v>2</v>
-      </c>
       <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38">
+    <row r="38" spans="1:10">
+      <c r="A38" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B38">
         <v>3</v>
       </c>
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
       <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39">
+    <row r="39" spans="1:10">
+      <c r="A39" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B39">
         <v>3</v>
       </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
       <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40">
+    <row r="40" spans="1:10">
+      <c r="A40" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B40">
         <v>4</v>
       </c>
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
       <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41">
+    <row r="41" spans="1:10">
+      <c r="A41" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B41">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
-        <v>0</v>
-      </c>
       <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="A42">
+    <row r="42" spans="1:10">
+      <c r="A42" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B42">
         <v>4</v>
       </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
       <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43">
+    <row r="43" spans="1:10">
+      <c r="A43" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B43">
         <v>4</v>
       </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
       <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44">
+    <row r="44" spans="1:10">
+      <c r="A44" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B44">
         <v>4</v>
       </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
       <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45">
+    <row r="45" spans="1:10">
+      <c r="A45" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B45">
         <v>4</v>
       </c>
-      <c r="B45" t="s">
-        <v>1</v>
-      </c>
       <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46">
+    <row r="46" spans="1:10">
+      <c r="A46" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B46">
         <v>4</v>
       </c>
-      <c r="B46" t="s">
-        <v>2</v>
-      </c>
       <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
         <v>42</v>
       </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
         <v>113</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>3</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>114</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
-      <c r="A47">
+    <row r="47" spans="1:10">
+      <c r="A47" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B47">
         <v>4</v>
       </c>
-      <c r="B47" t="s">
-        <v>2</v>
-      </c>
       <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
-      <c r="A48">
+    <row r="48" spans="1:10">
+      <c r="A48" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B48">
         <v>4</v>
       </c>
-      <c r="B48" t="s">
-        <v>2</v>
-      </c>
       <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49">
+    <row r="49" spans="1:10">
+      <c r="A49" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B49">
         <v>5</v>
       </c>
-      <c r="B49" t="s">
-        <v>0</v>
-      </c>
       <c r="C49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50">
+    <row r="50" spans="1:10">
+      <c r="A50" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B50">
         <v>5</v>
       </c>
-      <c r="B50" t="s">
-        <v>0</v>
-      </c>
       <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51">
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B51">
         <v>5</v>
       </c>
-      <c r="B51" t="s">
-        <v>1</v>
-      </c>
       <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52">
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B52">
         <v>5</v>
       </c>
-      <c r="B52" t="s">
-        <v>1</v>
-      </c>
       <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53">
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>113</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52" t="s">
+        <v>117</v>
+      </c>
+      <c r="J52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B53">
         <v>5</v>
       </c>
-      <c r="B53" t="s">
-        <v>1</v>
-      </c>
       <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54">
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B54">
         <v>5</v>
       </c>
-      <c r="B54" t="s">
-        <v>1</v>
-      </c>
       <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55">
+    <row r="55" spans="1:10">
+      <c r="A55" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B55">
         <v>5</v>
       </c>
-      <c r="B55" t="s">
-        <v>1</v>
-      </c>
       <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56">
+    <row r="56" spans="1:10">
+      <c r="A56" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B56">
         <v>5</v>
       </c>
-      <c r="B56" t="s">
-        <v>1</v>
-      </c>
       <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57">
+    <row r="57" spans="1:10">
+      <c r="A57" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B57">
         <v>5</v>
       </c>
-      <c r="B57" t="s">
-        <v>2</v>
-      </c>
       <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58">
+    <row r="58" spans="1:10">
+      <c r="A58" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B58">
         <v>5</v>
       </c>
-      <c r="B58" t="s">
-        <v>2</v>
-      </c>
       <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59">
+    <row r="59" spans="1:10">
+      <c r="A59" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B59">
         <v>5</v>
       </c>
-      <c r="B59" t="s">
-        <v>2</v>
-      </c>
       <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60">
+    <row r="60" spans="1:10">
+      <c r="A60" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B60">
         <v>6</v>
       </c>
-      <c r="B60" t="s">
-        <v>0</v>
-      </c>
       <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61">
+    <row r="61" spans="1:10">
+      <c r="A61" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B61">
         <v>6</v>
       </c>
-      <c r="B61" t="s">
-        <v>0</v>
-      </c>
       <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62">
+    <row r="62" spans="1:10">
+      <c r="A62" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B62">
         <v>6</v>
       </c>
-      <c r="B62" t="s">
-        <v>1</v>
-      </c>
       <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63">
+    <row r="63" spans="1:10">
+      <c r="A63" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B63">
         <v>6</v>
       </c>
-      <c r="B63" t="s">
-        <v>1</v>
-      </c>
       <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64">
+    <row r="64" spans="1:10">
+      <c r="A64" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B64">
         <v>6</v>
       </c>
-      <c r="B64" t="s">
-        <v>1</v>
-      </c>
       <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65">
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B65">
         <v>6</v>
       </c>
-      <c r="B65" t="s">
-        <v>1</v>
-      </c>
       <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
-      <c r="A66">
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B66">
         <v>6</v>
       </c>
-      <c r="B66" t="s">
-        <v>2</v>
-      </c>
       <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67">
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B67">
         <v>6</v>
       </c>
-      <c r="B67" t="s">
-        <v>2</v>
-      </c>
       <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68">
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B68">
         <v>6</v>
       </c>
-      <c r="B68" t="s">
-        <v>2</v>
-      </c>
       <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c r="A69">
+    <row r="69" spans="1:4">
+      <c r="A69" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B69">
         <v>7</v>
       </c>
-      <c r="B69" t="s">
-        <v>0</v>
-      </c>
       <c r="C69" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70">
+    <row r="70" spans="1:4">
+      <c r="A70" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B70">
         <v>7</v>
       </c>
-      <c r="B70" t="s">
-        <v>0</v>
-      </c>
       <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71">
+    <row r="71" spans="1:4">
+      <c r="A71" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B71">
         <v>7</v>
       </c>
-      <c r="B71" t="s">
-        <v>1</v>
-      </c>
       <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72">
+    <row r="72" spans="1:4">
+      <c r="A72" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B72">
         <v>7</v>
       </c>
-      <c r="B72" t="s">
-        <v>1</v>
-      </c>
       <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73">
+    <row r="73" spans="1:4">
+      <c r="A73" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B73">
         <v>7</v>
       </c>
-      <c r="B73" t="s">
-        <v>1</v>
-      </c>
       <c r="C73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74">
+    <row r="74" spans="1:4">
+      <c r="A74" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B74">
         <v>7</v>
       </c>
-      <c r="B74" t="s">
-        <v>1</v>
-      </c>
       <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75">
+    <row r="75" spans="1:4">
+      <c r="A75" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B75">
         <v>7</v>
       </c>
-      <c r="B75" t="s">
-        <v>2</v>
-      </c>
       <c r="C75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76">
+    <row r="76" spans="1:4">
+      <c r="A76" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B76">
         <v>7</v>
       </c>
-      <c r="B76" t="s">
-        <v>2</v>
-      </c>
       <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77">
+    <row r="77" spans="1:4">
+      <c r="A77" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B77">
         <v>7</v>
       </c>
-      <c r="B77" t="s">
-        <v>2</v>
-      </c>
       <c r="C77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78">
+    <row r="78" spans="1:4">
+      <c r="A78" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B78">
         <v>7</v>
       </c>
-      <c r="B78" t="s">
-        <v>2</v>
-      </c>
       <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79">
+    <row r="79" spans="1:4">
+      <c r="A79" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B79">
         <v>7</v>
       </c>
-      <c r="B79" t="s">
-        <v>2</v>
-      </c>
       <c r="C79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80">
+    <row r="80" spans="1:4">
+      <c r="A80" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B80">
         <v>7</v>
       </c>
-      <c r="B80" t="s">
-        <v>2</v>
-      </c>
       <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81">
+    <row r="81" spans="1:4">
+      <c r="A81" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B81">
         <v>7.5</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>78</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82">
+    <row r="82" spans="1:4">
+      <c r="A82" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B82">
         <v>7.5</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>78</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
-      <c r="A83">
+    <row r="83" spans="1:4">
+      <c r="A83" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B83">
         <v>7.5</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>78</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
-      <c r="A84">
+    <row r="84" spans="1:4">
+      <c r="A84" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B84">
         <v>8</v>
       </c>
-      <c r="B84" t="s">
-        <v>0</v>
-      </c>
       <c r="C84" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
-      <c r="A85">
+    <row r="85" spans="1:4">
+      <c r="A85" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B85">
         <v>8</v>
       </c>
-      <c r="B85" t="s">
-        <v>0</v>
-      </c>
       <c r="C85" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
-      <c r="A86">
+    <row r="86" spans="1:4">
+      <c r="A86" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B86">
         <v>8</v>
       </c>
-      <c r="B86" t="s">
-        <v>1</v>
-      </c>
       <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87">
+    <row r="87" spans="1:4">
+      <c r="A87" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B87">
         <v>8</v>
       </c>
-      <c r="B87" t="s">
-        <v>2</v>
-      </c>
       <c r="C87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88">
+    <row r="88" spans="1:4">
+      <c r="A88" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B88">
         <v>8</v>
       </c>
-      <c r="B88" t="s">
-        <v>2</v>
-      </c>
       <c r="C88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89">
+    <row r="89" spans="1:4">
+      <c r="A89" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B89">
         <v>8</v>
       </c>
-      <c r="B89" t="s">
-        <v>2</v>
-      </c>
       <c r="C89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90">
+    <row r="90" spans="1:4">
+      <c r="A90" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B90">
         <v>9</v>
       </c>
-      <c r="B90" t="s">
-        <v>0</v>
-      </c>
       <c r="C90" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91">
+    <row r="91" spans="1:4">
+      <c r="A91" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B91">
         <v>9</v>
       </c>
-      <c r="B91" t="s">
-        <v>0</v>
-      </c>
       <c r="C91" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92">
+    <row r="92" spans="1:4">
+      <c r="A92" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B92">
         <v>9</v>
       </c>
-      <c r="B92" t="s">
-        <v>1</v>
-      </c>
       <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93">
+    <row r="93" spans="1:4">
+      <c r="A93" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B93">
         <v>9</v>
       </c>
-      <c r="B93" t="s">
-        <v>2</v>
-      </c>
       <c r="C93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
-      <c r="A94">
+    <row r="94" spans="1:4">
+      <c r="A94" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B94">
         <v>9</v>
       </c>
-      <c r="B94" t="s">
-        <v>2</v>
-      </c>
       <c r="C94" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95">
+    <row r="95" spans="1:4">
+      <c r="A95" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B95">
         <v>10</v>
       </c>
-      <c r="B95" t="s">
-        <v>0</v>
-      </c>
       <c r="C95" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96">
+    <row r="96" spans="1:4">
+      <c r="A96" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B96">
         <v>10</v>
       </c>
-      <c r="B96" t="s">
-        <v>0</v>
-      </c>
       <c r="C96" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
-      <c r="A97">
+    <row r="97" spans="1:4">
+      <c r="A97" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B97">
         <v>10</v>
       </c>
-      <c r="B97" t="s">
-        <v>1</v>
-      </c>
       <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98">
+    <row r="98" spans="1:4">
+      <c r="A98" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B98">
         <v>10</v>
       </c>
-      <c r="B98" t="s">
-        <v>1</v>
-      </c>
       <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
-      <c r="A99">
+    <row r="99" spans="1:4">
+      <c r="A99" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B99">
         <v>10</v>
       </c>
-      <c r="B99" t="s">
-        <v>2</v>
-      </c>
       <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
-      <c r="A100">
+    <row r="100" spans="1:4">
+      <c r="A100" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B100">
         <v>10</v>
       </c>
-      <c r="B100" t="s">
-        <v>2</v>
-      </c>
       <c r="C100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101">
+    <row r="101" spans="1:4">
+      <c r="A101" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B101">
         <v>10</v>
       </c>
-      <c r="B101" t="s">
-        <v>2</v>
-      </c>
       <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
-      <c r="A102">
+    <row r="102" spans="1:4">
+      <c r="A102" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B102">
         <v>10</v>
       </c>
-      <c r="B102" t="s">
-        <v>2</v>
-      </c>
       <c r="C102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B13">
+  <conditionalFormatting sqref="C2:C13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2007,17 +2340,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B80 B81:C98 C99:C102 B99:B1048576">
+  <conditionalFormatting sqref="C2:C80 C81:D98 D99:D102 C99:C1048576">
     <cfRule type="containsText" dxfId="2" priority="2" stopIfTrue="1" operator="containsText" text="exercises">
-      <formula>NOT(ISERROR(SEARCH("exercises",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("exercises",C2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" stopIfTrue="1" operator="containsText" text="slides">
-      <formula>NOT(ISERROR(SEARCH("slides",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("slides",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B89 B90:C98 C99:C102 B99:B1048576">
+  <conditionalFormatting sqref="C2:C89 C90:D98 D99:D102 C99:C1048576">
     <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" operator="containsText" text="data">
-      <formula>NOT(ISERROR(SEARCH("data",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("data",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>